<commit_message>
Get daily reddit data: Tue Jun 18 08:09:00 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_23.xlsx
+++ b/data/2024_06_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3066 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1dil0jz</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>First time painting my toenails ❤️</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnm5ws72ba7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1dikp4s</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape are my nails? </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8njj58x6a7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1dikmc8</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Breaking nails</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dikmc8/breaking_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1dijrpe</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>New manicure</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv9chr0iv97d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1dijpvi</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Channelled my inner H0t Wheelz vroom vroom </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/548n9f1vu97d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1dijxzf</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Does anyone have experience with Mooncat polish?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dijxzf/does_anyone_have_experience_with_mooncat_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1dijsay</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>First time I tried acrylic 😅</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dijsay</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1dijd1m</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which style is best for a vacation? </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dijd1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1dij1ag</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>just learned how to do press ons, these are my very first sets in order! plz be kind im new to nails ❤️</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dij1ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1dihpxp</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel + UV light for long lasting press ons? </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dihpxp/builder_gel_uv_light_for_long_lasting_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1dihww4</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>I got my nails done with a cute light purple colour today, I know they’re basic but Y’ALL I got a surprise at bedtime. These nails G L O W in the dark so bright like I’ve got a black light in here or something. I had no idea that was a thing 😂</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dihww4</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1dij067</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oggsc63km97d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1diiolx</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">yellow for summer solstice on thursday </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diiolx</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1diid95</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Really enjoying the short nails for now 😌</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diid95</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1diiceq</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>So obsessed with this set I did on myself!</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lb909kdf97d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1dii4h3</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>One of my fav designs I’ve ever gotten 🍓</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a1glrfzc97d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1dihudr</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>got my nails done for eid!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dihudr</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1dihpsh</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>My first attempt at French tips!</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dihpsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1diez2w</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get rid of the hang? </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diez2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1dieie6</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Help please.</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wng5axkke87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1dih7cc</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just took off acrylics, how do I fix this and make my nails healthy again? The top layers are ripping off </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75pcmabn397d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1difl67</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Yellow 🌟 my shorties</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1difl67</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1dihl5o</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>DIY set</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dihl5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1dih1h3</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Simple but classy!</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dih1h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1digy5j</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Nails for vacay ☀️</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4j0k834197d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1digpg3</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Airbrush fan🥰</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d9cmndry87d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1digoth</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Look how much my nails have grown in 2 months! Can't wait to visit the nail salon next week</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s18msoily87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1dig18f</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Esto en nivelación con base! Que les parece esta opción?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doohjefes87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1dig0ld</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Sencillas que les parece ?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/telleaq8s87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1dig0bm</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Has anyone used CND Nail Strengthener RXx  ??</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dig0bm/has_anyone_used_cnd_nail_strengthener_rxx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1dig05l</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mucho color en estas uñas 💅 </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fe95pfa4s87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1difvb8</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Was going for mermaid vibes but is giving me beetle shell vibes - I'm still ok with that 🤔</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1difvb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1diff49</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diff49</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1dif4f8</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oau9otm8k87d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1diewmn</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>I asked my nail tech to match the off-white and gold in my bracelet</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5u4up39i87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1dief3r</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the colour </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0sdlt8od87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1diee6g</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink/ orange chrome </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diee6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1die83c</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Got a french manicure for the first time…</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xtvvqezb87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1die4i3</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Love the shimmer ✨</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yw1tlu43b87d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1die0zx</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Post no-chip damage or just bad?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1die0zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1die0zz</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Got a new set! WDYT?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1die0zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1didtfd</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>I finally found the perfect nude 😍</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1didtfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1didtdi</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>What colour nails would look best with this outfit for my friends wedding?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex4ak6pb887d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1dibvpl</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Nail broke really far in and now seems fused to side wall and not growing?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dibvpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1dictuo</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>My nail keeps breaking in the same location, can anyone explain to me why and how I can avoid?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0o44s2tz77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1didm1m</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Worked on my first bride this past week! Loved these white chrome bbs &lt;3</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vha9fvgg687d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1did8lv</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Help! How to acetone-soak my injured nail?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1did8lv/help_how_to_acetonesoak_my_injured_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1did5g1</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Dip powder opinions?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1did5g1/dip_powder_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1did2qf</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Plant Nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1did2qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1dicsyd</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>First post 💅</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dicsyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1dicihq</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>mix match nail art</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11nrb8d5x77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1dicie4</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Why is my polish not curing?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dicie4/why_is_my_polish_not_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1dich0o</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Powerpuff nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzttfbftw77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1dic6sk</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Modern Professional</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dic6sk/modern_professional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1dic3ro</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>another week, another set</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dic3ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1dibowh</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>One of my favorites!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wttie8xeq77d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1dibn52</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>simple cute color for summer or is this more springish ?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bq5se02q77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1dibilk</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>First Set of The Summer❤️🍓</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lvi7902p77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1dibgv9</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>tatts and nails and nature</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ecsnkorno77d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1dibftf</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>I loved this set🥺❤️</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76wng3oeo77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1dib9uc</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this normal? </t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dib9uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1diasga</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>My summer set= secured 💅🏼</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diasga</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1dialj2</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Magritte on GelX</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stj04zmph77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1diah3v</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Tried doing nail art for the first time! Need more practice (and definitely better equipment/polish), but I'm really happy with them!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n92bnntqg77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1dia5o9</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Hearts set</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dia5o9</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1dia0vg</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Think I’m getting engaged soon…got my first acrylic set!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry7gbdvcd77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1di9pcw</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>realistic-ish blueblerries (diy)</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di9pcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1di9jal</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Bold Color for Summer!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di9jal</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1di9i3r</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wedding nails 🤍 ombré French dip </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di9i3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1di9h5k</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Pride mani and pedi!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di9h5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1di9deh</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Pride Month Nails - Week 2</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1di9deh/pride_month_nails_week_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1di8zta</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Week two!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di8zta</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1di8hna</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>3D Chrome</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di8hna</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1di8hm6</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>First time I've polished my nails in years...</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia99rbkx177d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1di8d1f</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Press on questions</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1di8d1f/press_on_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1di89xo</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Added a chrome to a pink jelly gel and I love how it came out</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f7y3axb077d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1di83yn</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Pretty proud of this lava lamp moment. P.S: do not fear for my cuticles, just stained with the pink chrome</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di83yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1di7vvy</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Customer asked for 'pink glitter' &amp; here's what she got</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h9p9nv99t67d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1di7tt9</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Are there any options for adding length without acrylates?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1di7tt9/are_there_any_options_for_adding_length_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1di7osr</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>i feel so pretty &amp; girly 🎀</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di7osr</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1di65a5</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Nail ridges and hormones</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1di65a5/nail_ridges_and_hormones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1dhxw9a</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Pedicure bell post-toenail trauma</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ospmthjku47d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1di7dl6</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Barbie inspired nails 🌺🌊</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuvp801rt67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1di7a75</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Rate my drunken nails, accepting tips!</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di7a75</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1di76rc</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>back at it again 🥰</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di76rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1di74d6</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Black ombré chrome 🖤✨</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di74d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1di6q3e</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Moons and stars 🌙 ✨ 💜</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxc0m57vo67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1di6ecp</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>help! - retention</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di6ecp</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1di61qf</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>How I started vs. How it's going</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di61qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1di5ue3</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Beachy Nail Help!!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1di5ue3/beachy_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1di5tku</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>happy pride month 🌈</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5ljczn7i67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1di5mym</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Letting my little sister do my nails. She’s only been doing them for 6 weeks. So proud of her.</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu5f60kvg67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1di5i3z</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>My first time ever</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di5i3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1di5bpf</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Nail prep for peeling nails no efile</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1di5bpf/nail_prep_for_peeling_nails_no_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1di51p1</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Found my new favorite shop for manicures. (Bubble bath, chrome). Gel doesn’t break or start peeling off.</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4g992aic67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1di4yp2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I tried to make Doja cat inspired nail art ♥️ gel polish on natural nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e9r17keub67d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1di48r7</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>how would you caption these? 🎀💖</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di48r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1di4a3u</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>New Gel Manicure Set!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98yxu6uu667d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1di3x60</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Rainbow nails!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxgxr3t1467d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1dhqcmr</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>A student at a nail school filed my nails too thing and now the nail bed is flaking, how can I fix this?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dhqcmr/a_student_at_a_nail_school_filed_my_nails_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1dil7cj</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Pics do not do this polish justice. (You're Beautiful, Rogue Lacquer)</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dil7cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1dijrdv</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Cheap nail polish organization from Target!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dijrdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1diiv09</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>My first KBShimmer ✨🌙</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ah20ijfwk97d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1diir9z</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Holo nubs floating in the void</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8nk8y9qj97d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1diepo7</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>should i put a acrylic on a damaged nail?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diepo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1dic5zg</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>PFD - Hey Mercury, Can You Not?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dic5zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1dib3tb</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Help!! My nail always breaks on this spot since October last yr</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cfxboxol77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1di2nht</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Opal Vibes</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnma9tgsu57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1dig6bs</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>LBD - Fang's Real Name is Kevin</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dig6bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1dig3ti</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>I love Magnetics!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaj5p872t87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1dig0ip</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Fancy Gloss thermals are the best!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vkbf3y7s87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1difqo3</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Cirque’s Bisou Bisou is my new all time favorite polish</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krylu4sop87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1dif753</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>When the shade on your nails matches the shade of your shades…</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlrl4w7wk87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1dieqq1</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Pixie Party (the overlooked little sister of Fairy Dust)</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dieqq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1die62x</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Hard Reset</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1die62x</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1didmo3</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Looking for product recommendations based on my ideal characteristics</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1didmo3/looking_for_product_recommendations_based_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1diddhp</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>ABCs of polish. R is for Revlon!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s1yzrdd487d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1did3hb</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Matching my tumbler 💙💜</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iectrwwz187d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1did09y</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Best neon orange polish now that neon nacho (pictured) is no more?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/keaa7u09187d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1dict80</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Some ghetto first aid? 😂</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dict80</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1dic8cm</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>After seeing That Post, I was worried Sand Viper would look like bologna on me -- but no, omg it's a lovely shimmery nude blush. 🥹</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lpzp5ihtu77d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1dibpve</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Nightcrawler 🌃</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0n9mc6hq77d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1dibhwj</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Summer simple &amp; subtle</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dibhwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1diadgk</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Thank you all for the advice!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diadgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1di9x1n</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Trying out emily de molly!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di9x1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1di8t7u</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Uhhh... I added cat Frenchies with glow in the dark eyes 👀🐈</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di8t7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1di8l56</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Did my moms nails for her bday</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b495zkm277d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1di88jn</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Bluebell - INLP</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7eb8cl1077d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1di82t7</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Green Flake Bomb</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di82t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1di7yrt</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Really proud of my nails but just tested positive for COVID, so now you all are the only ones that get to see them.</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di7yrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1di7vpz</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Queen of the Valbaran Fae, my favorite magnetic polish</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jd4mpn75x67d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1di7o3e</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Bee’s Knees I Forgot to Breathe in golden hour light vs bright indirect light</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di7o3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1di7k9i</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>These are all different polishes - I think I have a type 😅</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp0hfyb0v67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1di7iqr</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Silent breath by edm</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b99gtiepu67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1di7chf</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Become The Art Yourself</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di7chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1di65s1</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Swatch comparison request: Phoenix's 'Boolba' vs 'Master of My Sea"</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1di65s1/swatch_comparison_request_phoenixs_boolba_vs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1di6183</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Ace and Aro: Pride Flags for Pride</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di6183</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1di5zxc</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Beautiful Forces 💜💙</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di5zxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1di5lza</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - A Pain in the Asteroid is so magical</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di5lza</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1di5dy8</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Mooncat Poseidon’s Prize 🌊🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbv8f911f67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1di5cdv</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Mooncat - Maelstrom 😻</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di5cdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1di4w6d</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Happy Pride Month! 🌈</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y2kjdbdb67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1di4dbz</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is your fav time saving tip/trick? </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1di4dbz/what_is_your_fav_time_saving_tiptrick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1di3m9h</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Chrome metal polish by snailworks</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8kjrkgs167d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1di2igu</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first Rogue Lacquer Polish! </t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di2igu</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1di1aa9</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Before &amp; After ft. a classic red 🌹</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzg89tdnk57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1di13jb</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Holographic nude for medium-toned skin</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka01r805j57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1di10v1</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Mermaid Nails</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxmc9t9oi57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1di0s47</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Shorties and Sour Apple Rings - Atomic Polish</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lui0yjjug57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1di0g1d</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Midnight Kiss vs House of Hades?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjz6o1wde57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1dhzfws</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bi Pride French Manicure 💖💜💙 </t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aaq1990s657d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1dhz5wh</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Hey Mercury, can you not?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dhz5wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1dhz50w</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Cockadoodledoom - Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dhz50w</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1dhxmoi</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>🪶🏳️‍🌈Two-Spirit Pride🏳️‍🌈🪶</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dhxmoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1dhxa21</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Tried a new nail tech this weekend and she gave me the prettiest nails I’ve ever had.</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et7spaf8p47d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1dhx3vo</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these overfiled? </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dhx3vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1dhwp9k</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Double Whammy of Nostalgia</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dhwp9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1dhv09d</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL I Will be Your Undoing! So pretty so sparkly! </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o9sssh7u147d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1dhugzo</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dhugzo/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1dht7ss</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>First time Gel X</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dht7ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1dikueu</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What a cute manicure</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5nq1cwn8a7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1dikdk1</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Some RUTO nails I made. Printed decals myself 💖</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6ujtipz2a7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1dih6d6</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>New nails🌟</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqgj0rsc397d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1digigc</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Hands up, this is a strobbery! 🍓🍓</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/247w3inxw87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1dieya5</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Sweet Nails</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs5odakoi87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1dieomy</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Recent press ons i made</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dieomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1diemjb</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Really happy with how this turned out. I have shaky hands, so sometimes I can’t get the results I want.</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okhzfbnlf87d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1dibly4</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Nails of the day 🎀</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz819lrsp77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1dialen</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Doctor Who nails I made today!</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8mpc1qoh77d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1dia44m</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Hearts set</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dia44m</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1di8x7w</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Honest opinions?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di8x7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1di8s8m</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Uhhh... I added cat Frenchies with glow in the dark eyes 👀🐈</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di8s8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1di6toj</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Stained glass inspired!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p9gcs1mp67d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1di5wmx</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>@nailedbymelon on ig did the cutest set ive ever had &lt;3</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di5wmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1di44o2</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Hand-painted nail art custom made by a fan . Stay tuned for Disney cat nail designs in the next update !</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mg7lsx0o567d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1di1j84</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>How to remove matte top gel</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1di1j84/how_to_remove_matte_top_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1di1764</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>My first stained glass set. I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di1764</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1di0e8s</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Working On structural manicures </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1di0e8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1di0cy8</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Cows and aliens for your day :)</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ap6r3resd57d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1dhwzax</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Super excited to be going back to Vegas to see Dead and Company so I decided to give you dye nails a try!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cknnaitim47d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun 19 08:08:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_23.xlsx
+++ b/data/2024_06_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:C639"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8611,6 +8611,2692 @@
         </is>
       </c>
     </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1djdq5g</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>A little French with a touch of 🌷</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djdq5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1djdi2g</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons I’ve made recently </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n72wkdm8gh7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1djdhzj</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Finally got the ombre down!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djdhzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1djcewv</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>What shape suits me?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djcewv</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1djc4qu</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Nail fungus or bacterial infection?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brfcyxtkzg7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1djb3e3</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>So pretty🥹🎀 custom press on nails ✨</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djb3e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1djag1i</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Sustainable Press-Ons/Nail Products?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djag1i/sustainable_pressonsnail_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1djad3j</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Toes to match ! I think i love these🫶🏻 done by me</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djad3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1dja9nx</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>First time having nails this long and doing press ons</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dja9nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1dja4dj</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Fresh grippers with my bestie 🥰</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dja4dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1dja474</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Ready for ur bday America 🤭🥂🎆 by @ nailsbyxoyanie</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iakwm5d0dg7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1dj9sc3</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>God bless nail stickers for giving me the floral nails of my dreams.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj9sc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1dj9nr1</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Something bright</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29xgvz5f8g7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1dj9i7y</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Is it normal for the tech to not treat nails before polish?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj9i7y/is_it_normal_for_the_tech_to_not_treat_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1dj9gn4</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Watermelon</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nujmfgig6g7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1dj9abr</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Summer refreshing vibe 🩵🤍🧡</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sos40eap4g7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1dj92mc</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Second attempt at gel x</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvxqvilm2g7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1dj92lr</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Loving my concrete colored nails haha</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj92lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1dj8jlw</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>I need inspiration</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj8jlw/i_need_inspiration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1dj8gxk</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>How are my first few applications?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj8gxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1dj8xp5</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>first time getting french tips!!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj8xp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1dj8x9n</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zebra nails on daughter </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj8x9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1dj8t50</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Newbie question</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5ma7pu30g7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1dj8s9f</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Gel on top of regular press on nails. </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj8s9f/builder_gel_on_top_of_regular_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1dj8oay</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>What's your opinion?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69yg5rluyf7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1dj7s6u</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Rip after letting it grow out :( what should I do</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj7s6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1dj83c6</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Nails I got vs nail inspo from Pinterest (@abbielouseee)</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj83c6</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1dj84p4</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Ever get your heart broken by your nails? 🙃</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkjzu4uqtf7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1dj838c</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>pink tips ! 🎀🌸</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj838c</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1dj81x8</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Que piensan de estas esculpidas en acrílico ! primer día de práctica…. </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj81x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1dj81hl</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>My Gel X nail set and my matching toes</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7hn7gmxsf7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1dj7m2d</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>So summery! 🍄🌻</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj7m2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1dj7kbh</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I let my nail tech do what she wanted today 😍</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj7kbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1dj79dz</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made this design for myself today! </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w44o1n8ulf7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1dj6zab</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Sonny Angel x Sanrio Nails</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsrq2ncajf7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1dj5zoy</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Do you re-use your Press Ons sets?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj5zoy/do_you_reuse_your_press_ons_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1dj5tjr</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>What is wrong with my nail?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj5tjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1dj60a3</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Lavender!🪻</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj60a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1dj5v3h</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Sangria</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sj1oh2kc9f7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1dj5szm</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>🐞Ladybugs Practice!🐞</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj5szm</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1dj53mm</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting Helluva Boss inspired nails 💅 Here is Blitzo! </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efckl4hx2f7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1dj5ink</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My partner and I got our nails done together! We both feel SO FABULOUS. </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj5ink</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1dj5565</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer fun </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2erx5qa3f7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1dj4zje</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Any Celtics Fans? ☘️🏆</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj4zje</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1dj4um5</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Sassy Sauce | Hella Handmade Creations | Be Dazzled</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj4um5</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1dj4k5b</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>If nautical mayhem is something you like...</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywck5v6eye7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1dj4c1t</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I told my tech I wanted pretty but with an edge. This is what we came up with. 🩷🤍</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qe4h4g9kwe7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1dj427z</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Pastel French Tips🩷💜🧡💙💛</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93ojqq0eue7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1dj40cy</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Natural nails?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj40cy/natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1dj2v48</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple sparkly nails. </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2v48</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1dj2sdw</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Feeling cutesy 💅🏻</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2sdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1dj2rh4</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Lines on nails?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2rh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1dj2pqq</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Need ideas</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj2pqq/need_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1dj2npq</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Black and white swirls on this magnetic grey</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2npq</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1dj2fdg</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Hibiscus nails🌺</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2fdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1dj2dmi</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Show me how grown out your nails are </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk2lkgx3he7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1dj1vbp</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>I think i found my perfect nude!!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj1vbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1dj1tqa</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Help with a nail drill</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dj1tqa/help_with_a_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1dj1q2k</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Bubbles in polish</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj1q2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1dj103n</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Fresh Biab Mani</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz7f807m6e7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1dj09sc</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Love these little dinos🥹</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uppdh9m41e7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1dj04vw</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Saving money by doing nails at home</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvvkoig40e7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1dizylw</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ate up some pride nails today! </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dizylw</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1dizptd</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>First Dip Powder…What Do We Think?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dizptd</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1dizlxo</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Neon Pink with White Marbling</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orn3ozl7wd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1diyi77</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>My first full French tip set [cursed pose]</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diyi77</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1diyiy9</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Flower nails! Inspo from kieraD on lemon8</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diyiy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1dizao6</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Can I use gel top coat over normal nail polish for the same/similar effect as gel polish?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dizao6</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1diz7pb</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diz7pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1diz0y6</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>It's giving....Happy Birthday to Me!!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diz0y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1diysoh</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>💙I love charms and stickers💖</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diysoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1diymwn</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Daisy nails!!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diymwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1diyl8l</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver sparkles and sand </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46lw4zplod7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1diyi8v</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>It’s been a week… is it reasonable to reach to the nail tech? they’re gel</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lx0suk1od7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1diy4b8</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Started doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exkqcim5ld7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1diy3if</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Just started doing my nails</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/357oxuczkd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1diy0xh</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Got my nails done right before vacation how we feelin? (bonus cat picture of her giving her opinion)</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diy0xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1dixvvq</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>I’m a beginner nail tech! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xthtqxcjd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1diws46</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>I hate my nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diws46</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1diwrn2</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Wedding nails done for a friend of mine! 🤍👰🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tszfdls7bd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1diwa9v</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>How to get Quinta Brunson’s natural looking nails?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diwa9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1diwjr8</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>My New color ❤️</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8dt58qj9d7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1diwews</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new set that’s giving bridgerton and arizona green tea at the same time </t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edfzfdhj8d7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1diwdzz</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Sunscreen prior to gel sets?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1diwdzz/sunscreen_prior_to_gel_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1diw4x8</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Are these as bad as I'm being told?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diw4x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1diw2cb</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>new set :)</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diw2cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1diqwwg</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there any real breathable nail polish? </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1diqwwg/is_there_any_real_breathable_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1diopod</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Went to a home based nail salon and this is what I got</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diopod</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1dimywy</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Can I restore the pink line below the free edge?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwuu4hw20b7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1dit13l</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>First time going to the nail salon: $50 for a French. Was I ripped off?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dit13l</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1divb0u</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Matte Love</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7i2f9u90d7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1diu738</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Ombre chrome nails</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy3p3yx2sc7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1dityj3</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>How do yall paint cute little flowers</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dityj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1diti54</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Love.</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diti54</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1dit20b</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>How do ya’ll feel about the Semi Cured Gel Nail Strips??</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dit20b</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1disysh</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Pinks nails and keyboard!</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xq6tfrcoic7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1disyww</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Can I use a semi-permanent nail polish without a primer/UV lamp?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1disyww/can_i_use_a_semipermanent_nail_polish_without_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1dish4x</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Ideas for next mani &amp; ??</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr61obr3fc7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1disc8t</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>press ons FTW</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2ltwp33ec7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1dirz3v</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>My nails are thin af</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dirz3v/my_nails_are_thin_af/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1djbkbm</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Easy tropical nail designs?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djbkbm/easy_tropical_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1djbhtp</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Glazed Donut nails using regular nail polish</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djbhtp</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1djasfr</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>can i paint press-on nails?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djasfr/can_i_paint_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1djaiaw</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>🌊 Thermal Nail Art at the Pool</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djaiaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1djac37</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Butter London experiences?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djac37/butter_london_experiences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1dja9gi</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Swatcha doin’?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dja9gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1dja49w</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Mushroom Mani 🍄</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dja49w</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1dj9w57</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Orly shipping?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dj9w57/orly_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1dj9c4d</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>mooncat goopy?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj9c4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1dj8m9e</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Nailon art ✨️ Sparkles and precious stones always 💎</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zytqsvdbyf7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1dj8k2i</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Mercury in Retrograde ✨</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj8k2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1dj7ath</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Eldritch Dreamworld - Femme Fatale</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj7ath</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1dj6a65</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Ran to Reddit when I saw these nails on a TikTok. Please identify this shade of red for meeee</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1dqdtx1df7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1dj4s4e</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hella Handmade Creations | Be Dazzled</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj4s4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1dj3bgd</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Mooncat Collaborates With ‘The Powerpuff Girls’ on Character-inspired Nail Polish Collection</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://wwd.com/pop-culture/new-fashion-releases/mooncat-powerpuff-girls-nail-polish-collection-1236437610/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1dj2d6c</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Favorite polish I’ve worn in a while! ILNP Euphoria</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2d6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1dj1c7l</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>“Let’s Bounce” from LynB Designs</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4v6i0589e7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1dj0jut</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Relic from my 2011 diary where I recreated my manicures! </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjb8oidw2e7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1dizs6g</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Pride in neon 🏳️‍🌈😎</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9znh8bjxd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1diyy4j</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Ballet slippers alternative??</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjd33m18rd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1diyoef</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>BKL - A Human Life is a Beautiful Thing Dupe?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kghqfbj9pd7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1diy649</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Which one to try first?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diy649</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1dixeh0</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Gel base coat, then regular polish and top coat?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dixeh0/gel_base_coat_then_regular_polish_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1divx4s</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>The holo is strong with this one</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1divx4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1divw85</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a very thick basecoat, to smooth dips on the nail </t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1divw85/looking_for_a_very_thick_basecoat_to_smooth_dips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1divtsj</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>My first duochrome -tip needed</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s88wg2l44d7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1dive9p</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Cute finds at TJ Maxx!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti9hicsx0d7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1diufvk</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish that looks like this does in the bottle? </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffseoddjsc7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ditys0</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Foaming at the mouth because this shade is sold out and I NEED IT 😫</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da4ewc8cqc7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ditvr6</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Freehand flowers!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lg3n3topc7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ditdn2</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>ILNP, Guest List</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ditdn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1dis4yk</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Beach vacation nails</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dis4yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1dir82f</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Opi adios bad nails, caio great nails + glazed n amused</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx3t46295c7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1diqsee</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Essie Jelly Gloss - Cheeky Jelly</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1xxc94r1c7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1diq2kv</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>ILNP OR HOLO TACO</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1diq2kv/ilnp_or_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1dipvum</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>🩵💚🏳️‍🌈Queer Pride🏳️‍🌈💛🩷</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dipvum</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1dip2z8</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Doo doo poopy nails that smudged while picking up dog poop</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dip2z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1diotkg</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>are regular nail files or glass ones better to make nails less sharp?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1diotkg/are_regular_nail_files_or_glass_ones_better_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1dimzwl</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new favorite topper! </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dimzwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1dimdc4</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these colors together </t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dimdc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1diln54</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>UK base coat recommendations please?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1diln54/uk_base_coat_recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1djduf8</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Cat eye gel</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1djduf8/cat_eye_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1djdn4j</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Pusheen press ons I made tonight</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8l5wk50ih7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1dj7kx1</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>It’s summer time! 🍄🌻</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj7kx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1dj6zwv</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Did my friends nails to match a tattoo she has</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj6zwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1dj64h5</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Hoppy To See You! 💕🐸</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqgns6anbf7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1dj5p3k</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>$1800 worth of nails</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw5v4rrw7f7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1dj59f4</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Fun stuff this week ✨💜</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj59f4</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1dj54d8</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting Helluva Boss inspired nails 💅 Here is Blitzo! </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlsl86543f7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1dj4hvn</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Technique help? </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj4hvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1dj2p0c</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and white swirls on this magnetic grey </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dj2p0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1dj1xg8</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>press on set by me 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hp6e1gnde7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1diyczv</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>I’m calling these “blueprint demon” nails [cursed pose]</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1diyczv</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1dixb9o</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Not as fancy as y’all’s, but I’m learning. 😊</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dixb9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1diwojl</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Cute little mermaid inspo nails :)</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xg5lmjkad7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1divthn</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Beginner nail artist! What do y’all think about these?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/583owai14d7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ditooh</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Aventure time</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y49pxx26oc7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1disppa</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Hers and His Press-Ons!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1disppa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun 20 08:09:39 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_23.xlsx
+++ b/data/2024_06_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C639"/>
+  <dimension ref="A1:C826"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11297,6 +11297,3185 @@
         </is>
       </c>
     </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1dk6bdb</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>My favourite set I've done so far</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk6bdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1dk5uor</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel top coat recommendations </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dk5uor/gel_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1dk4y2a</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>I know it's a little blurry but do you like it?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akdjzuct7o7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1dk4kiq</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4th set of diy gel x </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk4kiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1dk3thq</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Shout-out to bio-degradable press-ons. Does anyone here use them?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dk3thq/shoutout_to_biodegradable_pressons_does_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1dk315m</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Lil square set</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra7efyl0mn7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1dk2ati</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Best pressons for wide nail beds?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dk2ati/best_pressons_for_wide_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1dk1lg5</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>does anyone have any tips for getting stick-on nail adhesive off your natural nails 🥲</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dk1lg5/does_anyone_have_any_tips_for_getting_stickon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1dk1jbi</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Working on my PRIDE nails 🌈</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk1jbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1dk1i1j</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Feeling like a chili 🌶️</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grdknqip6n7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1dk1fkn</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Talk amongst yourselves &amp; Get your life right Boo</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk1fkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1dk1d4n</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>how much do you tip for a dip powder manicure?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dk1d4n/how_much_do_you_tip_for_a_dip_powder_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1dk19m0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Mocha ombré with hard gel and eye shadow!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rcfy8ch4n7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1dk0sr9</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>How to remove fake gel nails? (Without ripping off)</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dk0sr9/how_to_remove_fake_gel_nails_without_ripping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1dk0884</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Some nails i did today</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk0884</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1dk0248</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Daisy’s</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk0248</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1djzjwl</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome star alien holo nails. </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36u015dtom7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1djzfjl</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Help needed pls!!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djzfjl/help_needed_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1djze4s</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Gel polish base coat issues</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djze4s/gel_polish_base_coat_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1djz8az</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Kiara sky gel polish❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2n3ze7rlm7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1djz2gm</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>So tempted to replace my nails with these.</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9susyp8km7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1djyzwg</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>First time using polygel and foils!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1239rdiljm7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1djyxmu</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>So cute!! Are the charms too big?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/betterlovelyisabellinewheatear</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1djydwz</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried a new design. Thoughts? </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avbxfcf3em7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1djy5ya</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Rec for short, small press/glue ons?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djy5ya/rec_for_short_small_pressglue_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1djxyfs</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>My wife is ready for the summer! 🍊</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v13mu3qaam7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1djxwbc</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>thought yall would enjoy these pretty ones! 🖤</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djxwbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1djxkbf</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Summer Sunset Vibes 🌅🌴🦜🐬🐢🌿</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djxkbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1djxhev</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>pink french tips!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpcjbf1f6m7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1djxgxy</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Little clouds for Pride</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o66j06qa6m7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1djxgln</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Pink 🦩</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgxjqq986m7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1djx8ec</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Are the quicks of my nails unusually long?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxtdoqmc4m7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1djwu8t</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Is this apart of my cuticle?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3iziss31m7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1djwnpd</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Kitty cats</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbj7h59nzl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1djwmz5</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>High quality press ons?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djwmz5/high_quality_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1djwdwt</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Apres gel x - cut natural nails short before?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djwdwt/apres_gel_x_cut_natural_nails_short_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1djwaw1</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Did my nails last night:)) thought I would share.</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5cfrauwhwl7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1djwayq</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Not to shabby for a guy😝</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61nolvfuwl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1djw5s0</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>My cute new blue translucent set 🐟💙</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k09rqaovl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1djvwja</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Do you ever realize you hate your manicure and immediately redo it?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djvwja</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1djvvo9</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>My favorite set. What y’all think?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yacf9pogtl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1djvvnl</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre french m, coffin shape, acrylic </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywqhf9igtl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1djvm3e</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I have been doing my own press on nails and really like how these turned out!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djvm3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1djvlr8</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>The Nails Bae Chrome Tutorial</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t4a90n1crl7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1djv419</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Repair broken nail</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfyzwn6jnl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1djuzm8</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Broken Nail: Advice (content warning)</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djuzm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1djuo93</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>I’m not going for matte colors anymore 💝</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/046vv3c4kl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1dju6pb</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Should I pursue nail school?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dju6pb/should_i_pursue_nail_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1djufmv</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Healthy nails again 🥹</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ue0jycobil7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1djucr3</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>purple dip powder manicure</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxwxt4hohl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1dju6d8</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>First set in 2 years</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dju6d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1djta3b</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Suggestions/Inspo</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djta3b/suggestionsinspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1djsyys</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Simple Set</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wwnlgqc7l7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1djs5ri</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l18xket71l7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1djty1f</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>New Gel X Nails❤️</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un6iuwvnel7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1djtlzb</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Summer French tips!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n3l9go5cl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1djsq2h</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My birthday nails !!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vveutobh5l7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1djsdwg</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Gel powder vs acrylic powder</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djsdwg/gel_powder_vs_acrylic_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1djry39</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>💙 ILNP Pool Party 🩷</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djry39</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1djrodp</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>I am a 40 year old man with a 5 year old son who suddenly wants to paint his nails. I, I don’t even know where to start!</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djrodp/i_am_a_40_year_old_man_with_a_5_year_old_son_who/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1djrf7z</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Thank you u/fionnyn for letting me copy you 🥰 I'm not talented enough to do them myself though!!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djrf7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1djrcrd</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Blue squigglies.</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajjk6bs6vk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1djrbfh</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>My new nails for the Stevie Nicks concert in Chicago this Friday</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0f7tpxwuk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1djqzet</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>I'm obsessed with milky white 🤍🤍</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k923nsdhsk7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1djqcbq</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My favorite so far</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqhmxl2snk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1djqbb4</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Manicure</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djqbb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1djq9ly</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Apres Nails</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djq9ly/apres_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1djq8jz</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>My sister did her nails and I wanted to show them off</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mb9b2e0nk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1djq6f4</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Fruit nails I did on myself!</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djq6f4</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1djpxpa</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I can’t stop scrunching my hands to look at the magnetic ombré tips 😭</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djpxpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1djl0b0</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Skin issues</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djl0b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1djio0z</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My nail broke half way down with acrylics on, I’ve been soaking it off but what should I do</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef9u9jig1j7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1djejhw</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>How do I regrow cuticles?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djejhw/how_do_i_regrow_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1djgjoj</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Why are my nails like that (the top part)</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwr87xtbhi7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1djh0ty</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>I got acrylic overlay on my natural nails yesterday, and now my nails feel sore. Is that normal?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://imgur.com/ntHIr3U</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1djhw42</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>What's this thin line on my thumbnail. It hasn't changed in appearance since it has suddenly appeared 2 weeks ago. As far as I can remember I've had no injury on my thumbnail but I'm biting my nails since childhood. Could it be a splinter hemorrhage?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kixoiroui7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1djiv0k</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Natural Nail Update</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djiv0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1djjh1m</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Olive &amp; June Press Ons</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djjh1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1djm64w</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Should I get them filled in sooner or later?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jggvzb3psj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1djmz01</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Mexication Nails</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnk9xidpyj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1djnchy</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>I love my nail tech so much!</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djnchy</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1djpj26</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What designs are trending in 2024? </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djpj26/what_designs_are_trending_in_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1djph4b</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Glow in the dark for summer.</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djph4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1djp87u</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djp87u</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1djp838</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did them myself 😎 gel on natural nail </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djp838</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1djp3vc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Which shape looks better on me?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djp3vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1djok90</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Polish additive?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djok90/polish_additive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1djoe37</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Summer flavor</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbpynkn99k7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1djo61m</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>To those that moved to a new city: Did you switch nail techs?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djo61m/to_those_that_moved_to_a_new_city_did_you_switch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1djny9c</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Pride Style Nails. Using Sally Hanson's Gel style</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74vbvfv16k7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1djnu29</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>🤑💚✨</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djnu29</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1djnmhg</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>tried my best at doing stars lol still getting the hang of it</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djnmhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1djnbgc</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>June’s</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jx4b50oc1k7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1djn5nt</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beer and Cigarettes </t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djn5nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1djn4np</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbh2pfcxzj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1djmxgw</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>first time!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djmxgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1djmwp7</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will nails remain strong after structure gel? </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1djmwp7/will_nails_remain_strong_after_structure_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1djmf11</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Is anyone better at doing nail art on their dominant hand than their non-dominant?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djmf11</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1djm680</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Magneto nails</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ombydxrssj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1djlxtu</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Best full coverage nails for making press ons?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djlxtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1dk51yb</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>ILNP’s Kiss and Tell</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37umfgm49o7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1dk4h3x</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>You helped me find a shade before, what about this weird dark navy?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5379e7592o7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1dk4c1a</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Does anyone know a polish colour that matches this?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e7o7gul0o7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1dk3jbu</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KB Shimmer replacement brush </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dk3jbu/kb_shimmer_replacement_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1dk2hr8</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Tropical themed nails</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u63pq66ign7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1dk2cwa</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Working through my oldest untried ~ Cirque Coronation</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1drjgp35fn7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1dk1y9j</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Polish that looks like saphiret?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvslbgz2bn7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1dk1rbr</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Dance of the Moonlight Jellies 🪼✨</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk1rbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1dk1kid</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>misbehaving 😇</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk1kid</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1dk1h30</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Talk amongst yourselves &amp; Get your life right Boo</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk1h30</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1dk0sn6</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Aw Marbles!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2p2mhezzm7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1dk0nvc</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Tired of being a grownup</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w36vw8zqym7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1dk0nc0</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Shooting star! 💫</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk0nc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1dk04kz</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Gel nail brushes recommendations</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dk04kz/gel_nail_brushes_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1djzeqn</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help needed!!! </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djzeqn/help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1djz47u</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Breaking out this for summer</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q145465qkm7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1djyql3</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>💚🌲🍃🌳🦎🦠🪀</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djyql3</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1djypb9</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Blue Holo Skittle 🌌💙💎🩵</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djypb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1djxva7</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Summer Sunset Vibes 🌅🌴🦜🐬🐢🌿</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djxva7</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1djxdch</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Obsessed with layering things in jellies</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcbzkr5h5m7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1djwjfp</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Reds and Pinks</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djwjfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1djwi16</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Messed with these 2 colors and my nails came out great!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2yx1y9kbyl7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1djuzed</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>What can I improve on this male manicure I did by myself?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djuzed</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1djunqq</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Is this gel manicure sloppy or am I super picky?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djunqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1djuklw</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Got bored, therefore stickers</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/us819ahdjl7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1djubf2</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Nail broke</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djubf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1djtvct</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Swatch request: Essie separated starlight gold pearl nail polish</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djtvct/swatch_request_essie_separated_starlight_gold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1djttub</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>ISO: White-ish light lavender hue polish</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djttub/iso_whiteish_light_lavender_hue_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1djtt0s</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Incredible thermal by Fancy Gloss</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djtt0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1djtbcv</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>True Red Linear Holo?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djtbcv/true_red_linear_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1djspnh</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>ghosts of hecate perfectly matches my hydrangeas</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djspnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1djrw5w</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>💙 ILNP Pool Party 🩷</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djrw5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1djrrpp</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>In honor of the solar cycle</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hi36eas4yk7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1djrrt5</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>PFD Sunset Dust</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djrrt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1djroqq</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Where to find a polish this shade?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdtiqk5nxk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1djrhha</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Non-swatcher pics of Ethereal's 'Find me in the future'</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djrhha/nonswatcher_pics_of_ethereals_find_me_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1djr31r</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Unpacked My Polish Collection</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djr31r</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1djpozf</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>The Quintet</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djpozf</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1djp5og</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Midnight Rider Dupe</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djp5og</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1djp32e</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Sweet pea - ILNP</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etxyzutiek7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1djp2pe</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>What are some really good cuticle oils?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djp2pe/what_are_some_really_good_cuticle_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1djompm</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Touch of gold ✨️</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbj0ub04bk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1djocfg</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Pride Look</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pezgp44x8k7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1djo5z4</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>When it’s nail nail day so you just have to repaint your nails!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1sftxnn7k7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1djnt25</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>🤑💚✨</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djnt25</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1djng7j</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🩵💙🏳️‍🌈Aroace Pride🏳️‍🌈🧡💛 </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djng7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1djncbn</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>solar polishes = two different manis ☀️</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djncbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1djnbta</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>🪩🕺👻</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djnbta</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1djn1y1</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wc14wrxbzj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1djn0w3</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>house of hades 🌀</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpp59yk3zj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1djm506</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>A skittle gradient of some of the different Pride flags. ☺️🏳️‍🌈🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djm506</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1djlmq2</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Londontown Nail Veil #3 - Nope!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djlmq2/londontown_nail_veil_3_nope/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1djk3zv</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Jelly comparisons?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djk3zv/jelly_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1djjnb2</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sally Hansen's Insta-Dri Top Coat (in the red bottle) formula change...? </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qppz0q7o9j7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1djj6u3</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Rosewood and Pink lemonade </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djj6u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1djixcp</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Gorgeous but difficult to photograph Max Factor's Tahitian Sunset</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djixcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1djirnl</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Yellin’ yellow 💛</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihok4qwb2j7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1dji5lj</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Don't Get Another Dog 🐶</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dji5lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1dji3zm</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>How are you adding crystals to regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dji3zm/how_are_you_adding_crystals_to_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1djhu7w</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Cirque - Odette &amp; Fantasia</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djhu7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1djhcv3</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>BCB response</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kferrngnpi7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1djh426</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Kokoist summer red</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djh426</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1djgs7z</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Teal and gold</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djgs7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1djgqfe</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Bright red French tips 💅🌶️</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djgqfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1djg8ea</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - What a Marshmallow! 🐺</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djg8ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1djenbv</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you wrap the tip properly? </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1djenbv/how_do_you_wrap_the_tip_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1dj327o</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Rosarden sheer nude + Mooncat moondust</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z7cvtr8me7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1dk5zvi</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Garfield Cat</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk5zvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1dk53nx</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really wanted to push with freehand this time :) </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu63mjyp9o7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1dk21n9</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>May Nail Set Art</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk21n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1djz5bo</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>I'm in love with these</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/betterlovelyisabellinewheatear</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1djz0xq</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>First time using polygel and foils!</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ryzdct8vjm7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1djyynq</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>I pierced a nail. Lol</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph7wq5v9jm7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1djxoeg</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Summer Sunset Vibes 🌅🌴🦜🐬🐢🌿</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djxoeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1djwtk0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Super numb fingers but I love seeing my work all pretty and packaged. My type of dopamine</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djwtk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1djqyf7</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really happy with how these came out. </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bwnkwml6sk7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1djpz2b</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Some of my old jobs in a man</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3hfya82lk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1djpye1</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I make them to look better? They are press on </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fk1ufjxkk7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1djpfaf</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sexy snakes and chains 🐍 ⛓️‍💥 </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djpfaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1djmtn4</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Simple but cute 💅</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6det2a9mxj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1djmjfv</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>eyeshadow nails going patchy</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1djmjfv/eyeshadow_nails_going_patchy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1djme48</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>I did these stilettos</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djme48</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1djlpz0</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Nail salons in Tokyo</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqn88w2ipj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1djk32p</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Nails of the day</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyeftiq0dj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1djk1vv</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f00h25ircj7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1djj0rl</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Happy Pride Month 🌈</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em0zghnh4j7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1dje6xi</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Nail art ideas 💅✨</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dje6xi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun 21 08:09:40 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_23.xlsx
+++ b/data/2024_06_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C826"/>
+  <dimension ref="A1:C998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14476,6 +14476,2930 @@
         </is>
       </c>
     </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1dkyn4w</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo6zcqousv7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1dky71y</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>new sets i made!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dky71y</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1dky69t</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>I let my nail tech decide what design she should create on my nails. And here's the finished look, so gorg ✨❤</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mumvu42fmv7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1dkxrxm</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just checking for my anxiety </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkxrxm/just_checking_for_my_anxiety/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1dkxcht</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Alice in Wonderland Nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkxcht</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1dkx78q</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Beach set</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkx78q</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1dkp13k</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>PEDICURE CHAIRS WITHOUT PLUMBI</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkp13k/pedicure_chairs_without_plumbi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1dkna79</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Nails for my trip tomorrow</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkna79</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1dkmajf</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my nails done and noticed there is some separation between my 4 of my nails and the dip powder. </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w53hwhfyis7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1dkr0y5</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>“How do you do anything with those nails” answered! AND Long Nails Typing ASMR</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nd9l8yb4lt7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1dksi61</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>80’s inspired nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww40pj5wyt7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1dksy6b</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Help nail care</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4m49yzi13u7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1dkwe2p</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>grow out nails fast?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkwe2p/grow_out_nails_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1dkwg1i</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Nails done by my friend. I love it and wanted to share💟</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hw6po0lb2v7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1dkvwnj</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Good gift for ambitious 10 year old?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkvwnj/good_gift_for_ambitious_10_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1dkvwjf</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Made them myself! (Idk how to take aesthetic pics)</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkvwjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1dkvp8c</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Can I apply this under/before adhesive press ons?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0s3dp89uu7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1dkviah</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Is it normal for the nails on one hand to grow faster than the other?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkviah/is_it_normal_for_the_nails_on_one_hand_to_grow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1dkvasu</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Do you guys ever go out with just one hand done?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bsxuck1qu7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1dkv3mp</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>My post is getting binned by default. Help!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkv3mp/my_post_is_getting_binned_by_default_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1dkukjn</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Gel nails too thick?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hwc62qzpiu7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1dkujxb</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I want to do my own nails at home but..</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkujxb/i_want_to_do_my_own_nails_at_home_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1dkuchm</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Pink cloud nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkuchm</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1dku7zc</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Did my nails today 🤞🤩</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzq54mi7fu7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1dku7kv</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time getting nails and I'm so happy </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dku7kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1dkt5ua</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Question about acrylic nails!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkt5ua/question_about_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1dksqwm</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>What should I do about weak nails from gel?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dksqwm/what_should_i_do_about_weak_nails_from_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1dksgm8</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My newest set is giving me 70’s vibes but with the saturation turned all the way up❤️💜🩷🧡</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66lnie9hyt7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1dksfu2</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Can you color sculpting/3D gel?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dksfu2/can_you_color_sculpting3d_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1dksc5a</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Groovy</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dksc5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1dks5zs</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Longest my natural nails have been!!!’</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66qjfp7ovt7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1dkrtbz</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Natural nails with regular polish</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkrtbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1dkrnxl</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkrnxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1dkrfp2</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Could I pull off an oval/almond shape?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n12drpfyot7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1dkqpoy</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Does nail oil expire?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkqpoy/does_nail_oil_expire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1dkqjc6</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>2nd set of press on nails</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkqjc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1dkqflk</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>New set :)</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9p17sezft7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1dkpyso</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>new set 💅🏾</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1ojchd2ct7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1dkpv0k</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>First time using press ons,should I take them off?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkpv0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1dkprln</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>simple n pretty🍒🌹❤️🍓</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8selm2eat7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1dkplmr</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Everyone says oval/almond always looks best, but I feel like squoval suits me better? Thoughts?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkplmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1dkpkzm</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love a glitter flake nail 💅 </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gxhiulhv8t7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1dkpgjs</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Freehand angel eye butterfly</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkpgjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1dkovfp</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Are my cuticles beyond help?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkovfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1dkoq73</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Struggling to get any work done today - my nails are just too pretty and distracting! </t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkoq73</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1dkoq2q</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Piece of the top layer of nail came off - how to treat this? </t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkoq2q/piece_of_the_top_layer_of_nail_came_off_how_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1dkoiln</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Absolutely loved these</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdx6qrc40t7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1dkocpk</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">why do some nail techs seem annoyed at their clients? </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkocpk/why_do_some_nail_techs_seem_annoyed_at_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1dknu42</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Looking for fast cure monomer</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dknu42/looking_for_fast_cure_monomer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1dknooe</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Gel x by me</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dknooe</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1dkne6j</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>red tip french mani is so cutee!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkne6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1dkkmkn</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is my cuticle this white on the middle finger </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wepyq1r66s7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1dklsvn</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got an acrylic fill a few hours ago and not very satisfied with the result. I think the technician trimmed my cuticles too much. </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dklsvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1dkm76e</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>New nails, who this</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkm76e</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1dklvgf</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>What caused this row of skin stickning up?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dklvgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1dkjoyn</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Previous bad experiences, advice request</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkjoyn/previous_bad_experiences_advice_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1dkkp5v</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Switching Back to Normal Polish is Brutal…</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkkp5v/switching_back_to_normal_polish_is_brutal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1dkkxtu</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 4th set of DIY gel x nails </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkkxtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1dkkv5l</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Can you give me an idea of what I could do as a design on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqjg9lf08s7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1dkkut1</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pride nails </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkkut1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1dkk25g</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>My birthday set!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpanxnnv1s7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1dkjzz7</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>I love them ✨</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkjzz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1dkjck1</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pool water nails </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkjck1</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1dkjbqe</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>First time painting my nails, should I do it again? If yes, which colour do you think looks best?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uwokxcewr7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1dkj8gh</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in forever, is this an okay color for my skin tone? :P</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukytz0oqvr7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1dkj1ee</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Brittle nails and clipping</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkj1ee/brittle_nails_and_clipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1dkitts</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sailor moon inspired </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkitts</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1dkir7i</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>How to fix thin nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkir7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1dka2g4</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>why does my nail tech do this?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dka2g4/why_does_my_nail_tech_do_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1dkbbtf</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Problem.</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txdhzrp68q7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1dkikb7</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>What is going on here?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxyx0e0pqr7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1djziig</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Help! Nails falling apart!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djziig</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1dk528r</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Need help!! Should I do a 3d flower?? a cherry?? Dice??? I added inspo pics from Instagram for the flower.</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk528r</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1dkcuqz</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Brand recommendations for basic DIY gel mani?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkcuqz/brand_recommendations_for_basic_diy_gel_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1dkcwbw</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Did my nails literally last night, why did it fall off?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oms1mkfnkq7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1dkf693</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>The Nails Bae Double Glaze Chrome Set. How do you like it?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eneq64dn1r7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1dk33pz</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Winter Inspiration down under 🇦🇺</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3ris8psmn7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1dk1h7g</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Had my nails done for the first time in a while! Asked for a coastal vibe and got exactly what I asked for. 💛</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dk1h7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1djvf3q</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Poison nails</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1djvf3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1dkheje</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>The truth is out there</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkheje</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1dkhcql</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel vs Acrylic </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkhcql/builder_gel_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1dkh4hl</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Digging magnetic polish </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er6847r1gr7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1dkh016</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own dip nails with tips for the first time! </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq3j0xi5fr7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1dkgxq0</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Silver Pop Art Nails</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xftuauaner7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1dkgk9x</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Advice needed! I love them but I'm scared to put them on!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvj646ywbr7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1dkgaih</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>ready for summer 🍓🌸</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rym5dbvw9r7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1dkfo33</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching my nails with my kiddo's crocodile art </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkfo33</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1dkfb80</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Orange / Teal Aurora</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l3luk1n2r7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1dkf307</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello!! I wanted you to give me your opinion, I'm not convinced by the shape of the nails. I don't know if it's because of my big hands. </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5auisyzx0r7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1dkf2i5</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>My DIY birthday nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkf2i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1dkf0j8</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What would you do? </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkf0j8/what_would_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1dkeyl0</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>How often do you change your full coverage tips/Gel-X?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkeyl0/how_often_do_you_change_your_full_coverage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1dkcnhs</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make nail polish last longer? </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkcnhs/how_to_make_nail_polish_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1dkcl8t</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Do pedicure places hate male clients?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkcl8t/do_pedicure_places_hate_male_clients/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1dkcgyx</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Fresh mani ft. week one of not cutting the proximal nail fold</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkcgyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1dkccys</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Hoping for the best</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1udmi0iigq7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1dkc6le</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Filing Gel</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkc6le/filing_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1dkbuwg</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>First time using Gel</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkbuwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1dkbo4e</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Top coat to extend wear?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dkbo4e/top_coat_to_extend_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1dkbjh0</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail shape? </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8kv3mdy9q7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1dky0s1</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Mooncat - Treachery in the Blue</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw83b56qkv7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1dkxxku</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">playful pink mani! 💕 (+bonus: my brand new engagement ring 🥰) </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbv42dumjv7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1dkw440</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>My friend overfilled my nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkw440</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1dkv2at</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>First post and first time getting nails done professionally!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkv2at</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1dkuwhc</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>How to safely use bobby pins while protecting manicure?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkuwhc/how_to_safely_use_bobby_pins_while_protecting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1dkujvh</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Best one coat black and white</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkujvh/best_one_coat_black_and_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1dkudxs</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>They've come a long way ✨</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkudxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1dktu33</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>🍊🐈 🧡i would die 4 u 🧡🐈🍊</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dktu33</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1dkthu7</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Happy pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkthu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1dkth4p</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Matching my strawberry Dr. Pepper</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkth4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1dksza9</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>festival nails 💅</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dksza9</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1dksxll</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Thoughts on Essie’s Treat Love &amp; Color?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dksxll/thoughts_on_essies_treat_love_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1dkssmw</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Gooey polishes? Thinner vs. Acetone</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkssmw/gooey_polishes_thinner_vs_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1dksk3u</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Dupes for the og formula/release hard candy polish?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dksk3u/dupes_for_the_og_formularelease_hard_candy_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1dksbef</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Magnetic toppers [US]</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dksbef/magnetic_toppers_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1dkrz4q</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>First time in over 2 years!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwl6wj3wtt7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1dkre6o</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>First time glazed donuts!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkre6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1dkqpr0</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>more pride nails :-) (long/short)</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkqpr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1dknzgk</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>I’m just really excited and have to share my haul</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dknzgk/im_just_really_excited_and_have_to_share_my_haul/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1dknx06</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>LA FRENCH NUNCA FALLA 😍</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecif1ooavs7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1dkhhw4</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Overfiled because of leftover polish</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkhhw4/overfiled_because_of_leftover_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1dkafl3</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>So what if green makes my hands look red. 🤷</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkafl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1dkqre6</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Come On!!!!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkqre6</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1dkqpxg</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Do you match your pedicures with your manicures? I don't want to chance my pedí so often but it bothers me that hands don't match 😭</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fz2dg6bhit7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1dknx8n</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Lightness and Darkness</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dknx8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1dkno87</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>My Favourite Green</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkno87</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1dkmhbp</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> So good!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkmhbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1dklwsc</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid Bait but warm-toned? </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dklwsc/mermaid_bait_but_warmtoned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1dkltlt</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Any dupes for the green flaky polish in this pic?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs4mi5n6fs7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1dklm8q</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>please help! What nail colour would look best with this dress?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2nmmcymds7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1dkl3qb</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>A pain in the asteroid ☄️</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkl3qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1dkkm3w</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>A nice neutral is my safety blanket</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkkm3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1dkkjkb</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>had to do a chop 💔</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkkjkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1dkkcpk</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>The number of unsolicited messages I've gotten from creepy dudes with a hand fetish is honestly really offputting</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkkcpk/the_number_of_unsolicited_messages_ive_gotten/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1dkjwk6</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Pride in primary colors 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkjwk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1dkiwk4</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Neon shorties for summer ☀️</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkiwk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1dkisob</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Squirtle nails🫧💧</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkisob</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1dkhtrl</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Regrowing nails entirely?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkhtrl/regrowing_nails_entirely/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1dkhm5t</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Watch a Nail Tech Turn Her Nails into a Masterpiece! Video in the comments.</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81ztg145jr7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1dkhi5p</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>How do you shake your nail polish bottles?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkhi5p/how_do_you_shake_your_nail_polish_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1dkhax1</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Some glitter got into my acetone and it looked magical</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k55ytw3chr7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1dkh41a</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Colorful Jelly Sandwich</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtcg9txjfr7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1dkfnrq</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Bi-moon Pride Nails</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkfnrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1dkflfg</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Color Club Neon Comparisons?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkflfg/color_club_neon_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1dkfhbl</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the shelf life of thermal nail polishes. </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkfhbl/what_is_the_shelf_life_of_thermal_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1dkffzi</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Thermals</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkffzi/thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1dketgf</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Treachery in Blue paired with the Crystalline topcoat has me in a chokehold 💙</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cevjg0yyq7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1dkeru2</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>an Aphrodisiac Treachery</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkeru2</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1dke83m</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>🩷🩵🏳️‍🌈Demigender Pride🏳️‍🌈💛🩶</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dke83m</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1dke536</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>French twist</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75up4t7ytq7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1dkdala</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>periwinkle nails</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnwa2vdlnq7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1dkcj5q</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>MC "a midsummers dream" for midsummer tomorrow</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkcj5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1dkc96d</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Swatch Request: It's Brittney, Beach vs Low &amp; Be Bold</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkc96d/swatch_request_its_brittney_beach_vs_low_be_bold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1dkbael</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Nail Polish no contact</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dkbael/nail_polish_no_contact/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1dkb8ff</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Dont do my nails very often but pool nails are a must every summer</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkb8ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1dkak46</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Barbie nails for my birthday 💜</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkak46</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1dk9z3b</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Preparing for Polish &amp; Beauty Expo 2024?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dk9z3b/preparing_for_polish_beauty_expo_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1dky1p4</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Porcelain Painting</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyokkn22lv7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1dkv8oj</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>This month's set 🥰</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9su37zfpu7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1dkt84d</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>So that the gradient looks good on me, I apply the polish with my FINGER 🤯</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65qqx3on5u7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1dkrffg</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>I tried crystals for the first time!</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjtokotvot7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1dkq3ht</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>My nails have made me happy all week</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkq3ht</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1dkosch</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>My first time</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b83ntwrb2t7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1dkjtuu</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Nails for a greece vaca</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkjtuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1dkjnue</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>My DIY birthday nails</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkjnue</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1dkhufz</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of my nails? </t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0snb04glr7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1dkh5bq</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>The truth is out there</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkh5bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1dkf3zq</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my new work! </t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8xusvm51r7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1dkeaoq</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Just started gels</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkeaoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1dkc3px</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">90s nails match my Lithium </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkc3px</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1dkaq2b</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icy summer nails 🧊 </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkaq2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1dkac6t</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Practice Nail Art</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/769psdugzp7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun 22 08:09:02 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_23.xlsx
+++ b/data/2024_06_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C998"/>
+  <dimension ref="A1:C1164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17400,6 +17400,2828 @@
         </is>
       </c>
     </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1dlq5zy</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I miss my sparkly nails </t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlq5zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1dlpp1j</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>A lighter ombre than usual</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g37ahz7hm28d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1dlpnmk</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Nail glue</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlpnmk/nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1dlopui</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something fun for summer ☀️ </t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlopui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1dloj5w</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Gel extensions/ gel manicure and working out</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dloj5w/gel_extensions_gel_manicure_and_working_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1dlo5m1</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>opinions on nail strengthening polishes</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlo5m1/opinions_on_nail_strengthening_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1dlnza0</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>I get all these cute ideas then I just go back to my usual 😅</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8rrwggd228d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1dlnxs2</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>hello kitty summer</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2h7z290228d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1dlnuso</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Some psychedelic nails 👽</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlnuso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1dlnmqm</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lilac and natural color, a beauty!!! </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09u8wnqny18d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1dlnchg</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>I think this is the longest my natural nails have ever grown! And they’ve been so strong too! But I broke one nail on my other hand while doing Pilates 🥹</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlnchg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1dln9ju</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Obsessed with this press on set</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dln9ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1dln9b7</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail spots </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xna6orkmu18d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1dln8l5</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Confusion on What to Get</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dln8l5/confusion_on_what_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1dln3g9</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Dip vs anything else</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dln3g9/dip_vs_anything_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1dlkgih</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Nails one week after a horrible tech and after once another tech fixed them.</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlkgih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1dlmn47</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I’m just go proud of this toe transformation I did 🥺 (NOT FUNGUS)</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlmn47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1dlmn9h</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blush nails </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93u6dzcgo18d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1dlml3l</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Did these today. Dont look too close.</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlml3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1dlljp9</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>sticky tab recommendations?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlljp9/sticky_tab_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1dlm4in</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Ocean ready</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo420634j18d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1dlld3x</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>any feedback on how to improve?  Did Gel x on myself, first time - took almost 3 hours ... and not super happy with how it looks</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80a0wm9eb18d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1dllb9s</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Summer Set</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dllb9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1dlkn4m</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>I fell in love again</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g5fq6jv418d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1dlk9py</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Fave set</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlk9py</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1dljylg</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>What to expect when getting nails done for the first time?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dljylg/what_to_expect_when_getting_nails_done_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1dljaer</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>I broke my nail and don’t know what to do</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dljaer</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1dljosk</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Midnight Snack</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dljosk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1dlj8ok</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frenchies </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inz1cvufr08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1dliqui</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>I need some feedback (please read the post)</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dliqui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1dlj1pa</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlj1pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1dliyxm</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Ombré nails with water drips 💦</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/veolomgxo08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1dlitmk</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Let's talk about discrimination</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlitmk/lets_talk_about_discrimination/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1dlijbt</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Can you file dip after you’ve left?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wvhacl7l08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1dliagt</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Based on inspo from this sub!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8so5gr33j08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1dliadx</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Is UV nail lamp damaging to the eyes?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dliadx/is_uv_nail_lamp_damaging_to_the_eyes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1dli5u5</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Just got some new gel polish in, couldn’t pick just one</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voufzduxh08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1dlhzz3</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Color: I want Kisses.</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlhzz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1dlhxir</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Least favourite nails</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlhxir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1dlhmcz</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>It never dries (regular nail polish)</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlhmcz/it_never_dries_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1dlgp4k</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Nailed it!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g5di2wk508d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1dlh410</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Short nails club</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlh410</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1dlgqck</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails ready!! </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh37gryu508d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1dlebg2</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>help! nail splitting?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/531uvaimmz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1dlgdmq</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>How do I ask for this? Inspo from insta @tgbacdemy</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caykhg1y208d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1dlg4q1</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>I️ don’t often get my nails done, but I️ do love it when I do. 🖤🩷</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql6x860w008d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1dlg34z</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Did my sister's nails</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlg34z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1dlg01w</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Just finished this weeks mani 💜</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlg01w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1dlfk9a</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>A beauty that orange babyboomer 🍊</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be5p2audwz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1dlfjqa</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>beautiful💙</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdx6j9cawz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1dlfi1w</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Press on nails that match Cliniques Black Honey?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlfi1w/press_on_nails_that_match_cliniques_black_honey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1dlfena</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Citrus Nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlfena</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1dlf1zs</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>my 4th of july nails! 🇺🇸🦅💥</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro9m55zdsz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1dlek9x</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Took my grandma to get her nails done 🥰 she looks amazing in pink 💝💖🌸</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlek9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1dldmh8</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Quality short press on nails?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dldmh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1dldlg2</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>how do you keep this from happening when filing your nails?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxyc94m2hz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1dldy8m</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Why can’t we include the knees??</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dldy8m/why_cant_we_include_the_knees/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1dlds4f</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Which nail drill is better?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlds4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1dldpx2</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>in love with my new set</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dldpx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1dlamsr</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Not sure what’s going on with my nails (read caption)</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqasa78juy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1dldb4a</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>summer citrus set! 🩷💛</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dldb4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1dlae1c</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>should i get this looked at</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4wrilmpsy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1dld8ss</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>A simple set of press ons I made just for fun.</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m19rm4y9ez7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1dld6nk</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Got a pedi for the 4th 🎆</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/521ij99tdz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1dlcori</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>HELP!!! 🚨I have a First Date Tomorrow &amp; I need Nail Advice!!!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpjnjh13az7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1dlcunq</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>press on nails!</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cnbu35w8bz7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1dlcyml</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Why do I always have this red line around the bottom of my nails?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4flim236cz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1dlcql2</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Perfection. My Nail Tech Gets the Job Done EVERYTIME💗</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlcql2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1dlcliw</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Would love criticism!!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlcliw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1dlckc7</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>I have my first ever appointment booked tomorrow. Do I clip my nails or not?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlckc7/i_have_my_first_ever_appointment_booked_tomorrow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1dlcf57</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Gel polish wrinkling</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am5d2r428z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1dlce4a</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>First time ever doing press on's!!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ek3por7z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1dlcbwf</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqqah0hd7z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1dlc1pw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnd0psl65z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1dlc1jd</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Wavy summer</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx6umxy45z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1dlc1cd</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>New set 🤎</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an5v4m835z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1dlbyjm</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Didn’t think I could like my nails this short!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlbyjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1dlbkir</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Apres/Gel X white base with chrome/iridescent pink finish </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6jp7z1ij1z7d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1dlbcg1</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>I updated my milky white nails and add some glitter for a fun summer look ✨☁️ Glitter fade yay or nay? 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlbcg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1dlbawp</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>First Summer Set 💙💜</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlbawp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1dlb1ep</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>My graduation nails!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zuwhkkjxy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1dlaz4m</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Birthday nails✨🔮</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr2oyoz1xy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1dlam11</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Vacation nails that my nail tech did. I love them so much!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlam11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1dlad7k</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Press on nails recommendations</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlad7k/press_on_nails_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1dl9pw6</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail stamping </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmq2qhyqny7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1dl9dej</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fixed nails </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl9dej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1dl4vfq</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>How can I DIY repair a cracked nail before my nail appointment?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dl4vfq/how_can_i_diy_repair_a_cracked_nail_before_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1dl8xyk</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>yellow and almost black nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze1hkdkvhy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1dl8yu8</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>help learning how to find a safe nail tech</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dl8yu8/help_learning_how_to_find_a_safe_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1dkzx2c</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Love my new cloud nails! ☁️✨</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q32ugzo99w7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1dl01cq</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>PINGU NAILS</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl01cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1dl08a8</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Genuinely, how do you use magnetic polish? I don’t understand how to use the magnet. Sometimes it pulls the shimmer away and sometimes it pushes it away. How do I intentionally position the magnet to pull and push the shimmer?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dl08a8/genuinely_how_do_you_use_magnetic_polish_i_dont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1dl1mno</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>What type of nail should I get?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dl1mno/what_type_of_nail_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1dl2y8t</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>what kind of pedicure does @talitacardozo on tiktok do?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl2y8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1dl8em7</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gelx allergy but not Acrylic </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dl8em7/gelx_allergy_but_not_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1dl8r36</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>I spent 3hrs fixing my nails after seeing a beginner nail tech</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl8r36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1dl8u8k</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>23 year old nail tech that loves art!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl8u8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1dl8i1b</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cant go wrong w chrome frenchies </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aael8xjhey7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1dl87zh</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My chrome nails </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efuk1baecy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1dl7wa5</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help, I’m begging you!! (It’s not like nasty or anything, I just tried to post already and it didn’t, I assume I needed NSFW.) </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl7wa5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1dlnhua</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>looking for a color like this!! (nude with a hot pink-ish/red shimmer)</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlnhua/looking_for_a_color_like_this_nude_with_a_hot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1dllqv2</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Palate cleanser mani, but make it ✨glittery✨</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dllqv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1dlllbd</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>How do we feel about No Room For The Blues for the solstice? ☀️ 🦋</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcga6otvd18d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1dll4xq</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Sheer + Opal Glitter</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dll4xq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1dlkmnu</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Dracula Nails</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sp9wbqq418d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1dljwsm</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>What is your go-to method for destaining/brightening your nails some? I've done dark colors the last couple times, I DO use base coat, but I'd like to lighten these a bit if possible?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di6r1uprx08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1dljqje</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Midnight Snack</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dljqje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1dljd07</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Mint Julep as Inspiration</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd06zjvjs08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1dlj1ip</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Wanted a nude palate cleanser…with a little flash!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ij71l8jlp08d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1dlhpeb</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Lumen - Glass Star</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4myqkhj0e08d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1dl7nb5</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seeking translucent pink gel polish-salon quality </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dl7nb5/seeking_translucent_pink_gel_polishsalon_quality/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1dlftm7</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cracked Skittle 💄 </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr14bc2hyz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1dlflky</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Summer Solstice magic</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlflky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1dlfimp</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>needing suggestions for colors</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qildl671wz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1dlf1f9</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Bit of a disappointment w/ Essie</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlf1f9/bit_of_a_disappointment_w_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1dlf0fk</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Butterflies and Stars!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlf0fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1dleqvs</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Cirque lagoon + Poparazzi Glass Ceiling</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aybkwcvpz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1dlek1a</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>for anyone whose bought mercury's tears from mooncat recently</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlek1a/for_anyone_whose_bought_mercurys_tears_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1dldt8d</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>To chop or not to chop?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dldt8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1dlds59</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Morgan Taylor June Bride</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlds59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1dldnxy</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Pride themed polish collections?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dldnxy/pride_themed_polish_collections/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1dlbzpq</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Demi nails! </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe7jl84q4z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1dlbrob</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>First Orly that’s not base or top coat, loving it!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlbrob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1dlbe6s</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Beach Ready Mani</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fqrtof50z7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1dlb8s2</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Looking for strong, temporary press-on adhesive</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlb8s2/looking_for_strong_temporary_presson_adhesive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1dlazqv</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Dupe Request: Melange by Illamasqua, teal with fine gold flecks</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlazqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1dlakru</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone have the DRK Hydrangea kit? </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlakru/does_anyone_have_the_drk_hydrangea_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1dlakri</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Can someone help me find this color? (Pics below)</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlakri</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1dladj5</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Something something harlequin</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dladj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1dlab2e</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>A Most Destructive Melody</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlab2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1dl9pgj</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Any reccs for an off-white, cream, or ivory colored creme polish?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dl9pgj/any_reccs_for_an_offwhite_cream_or_ivory_colored/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1dl96r2</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈LGBTQIA+ Allyship🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl96r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1dl8a5z</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Getting caught up with my manis 💅</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl8a5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1dl80wl</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Power Mooncat</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1bn9n4xay7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1dl6v2b</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Pastel holo Bi Pride nails 💗💜💙</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl6v2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1dl6uu0</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Mooncat at a Dominican Nail Salon</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dl6uu0/mooncat_at_a_dominican_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1dl6kht</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>i love my new nails 🙈</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl6kht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1dl6hnq</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>my nails last week 🥰</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl6hnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1dl6awz</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lush - Polished for Days </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl6awz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1dl5kpf</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Newly re-obsessed with toppers</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl5kpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1dl4ef6</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Beautiful color, but…</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5olgg2hvix7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1dl3a7j</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Sweet Pea is so hard to capture but here’s my attempt</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fnqtt399x7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1dl1yxp</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>You guys made me do this</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl1yxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1dl0hg4</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>ILNP - Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl0hg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1dl0cnc</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>r/RedditLaqueristas Moderator Announcement concerning creeps in order to make the subreddit safer</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dl0cnc/rredditlaqueristas_moderator_announcement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1dkzzw3</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>New nails for eras tour</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dkzzw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1dlmcxn</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>FREESHAVOCKADOO! 🥑💕</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6whw15hl18d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1dllrb1</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Flowers 🌺</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dllrb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1dllnlq</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Billie Eilish HMHAS album nail art </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dllnlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1dlj08h</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Did these marbled acrylics</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c5szoc9p08d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1dliuxb</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Summer seashell nail art!</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ya35cz2un08d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1dli1vo</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dumb Question </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dli1vo/dumb_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1dlg10t</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Did my sister's nails</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlg10t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1dlezqh</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>On the scale of 1 to 10 how bad did I mess up the butterfly?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlezqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1dleym9</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Butterflies and stars!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dleym9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1dleol4</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Casual-Elegant Nails (2.5 hours) 🌿</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dleol4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1dle3yh</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>What do you think of these "blood nails"?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz7wtbxzkz7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1dldctu</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>summer citrus set! 🩷💛</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dldctu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1dla9og</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Getting back into nail art</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dla9og</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1dl9syg</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>🌶️🌶️🌶️</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1e0k5jeoy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1dl9i6k</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>My first time using 3D gel</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl9i6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1dl917j</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Beginner Gel Art</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl917j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1dl8qgl</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>ART INSPO @sinvnails</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ythp9rfdgy7d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1dl5n9u</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Hi, take a look at my new nails. I love them so much!</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq5zoq7qsx7d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1dl2svu</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Did my sisters nails for her graduation 💜✨🌌</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl2svu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1dl17wj</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Love how these came out!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dl17wj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun 23 08:07:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_23.xlsx
+++ b/data/2024_06_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1164"/>
+  <dimension ref="A1:C1327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20222,6 +20222,2777 @@
         </is>
       </c>
     </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1dmfwyn</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Damaged nails?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dmfwyn/damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1dmfz03</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Does this color wash out my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/seesvl7un98d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1dmfp2j</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥳🍒</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhrjf36hk98d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1dmfnch</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>how to take care of natural nails?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dmfnch/how_to_take_care_of_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1dmf9xk</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>i’m new to making press ons. i really like this set i did</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmf9xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1dmeij9</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Recent sets :)</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmeij9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1dmecv6</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need tips/advice </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmecv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1dmdy7e</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>went a little outside my comfort zone.. I’m not mad about it ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmdy7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1dmdv15</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Trying something new</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqjzncjdz88d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1dmds7a</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">❤️ </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ga2v1piy88d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1dmdl9w</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Any press on recommendations for my spoon thumb girlies??♣️🥄</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydfeo60kw88d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1dmdd3e</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Is it normal to charge for multiple colors?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dmdd3e/is_it_normal_to_charge_for_multiple_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1dmbxsm</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for “Nurse Nails” inspo </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dmbxsm/looking_for_nurse_nails_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1dmbyug</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the best I’ve ever done my nails! </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmbyug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1dmb2ks</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>First time getting my nails done. Does this look right?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmb2ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1dmbbrz</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>The only colour I like for my nails but I don't think it suits for summer nights</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mhqruwe988d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1dmazy3</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Neon leopard print</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04tdobu7688d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1dmaup6</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My vacation nails from the last 6 months </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmaup6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1dmap1q</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunset Chrome </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja7mmhga388d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1dmaln7</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Sha'Carri Richardson's Nails</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rny9l4mc288d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1dmajtw</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>How to remove set gel?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etdza6cw188d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1dm9zhx</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pearly pink </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm9zhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1dm9t15</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I've been doing my own nails for 2-3 years now</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm9t15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1dm9ha0</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A difficult typeface to make </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izwpadrtr78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1dm9h0e</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>I’m in love!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5at0rcrr78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1dm96vw</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>This set was only $65</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm96vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1dm8c9w</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>3 years worth of acrylic damage. Any advice how to fix it?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm8c9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1dm92mf</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Every now and then, a basic polish is what I need. </t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sanssau4o78d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1dm7s4y</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Apex too thin?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux88nopsc78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1dm8uhj</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Done on myself 🩷🖤</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00xr9773m78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1dm8enb</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Does builder gel expire?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm8enb/does_builder_gel_expire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1dm8cu0</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>New girly nails!!! So in love</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm8cu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1dm87q8</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Russian manicure ✨💅🏽✨</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm87q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1dm87le</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Vaca nails ready ✅</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8vmi4ajg78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1dm865s</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This month's colour </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm865s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1dm8212</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this new set </t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm8212</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1dm8067</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Pixar set for upcoming Disney trip</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsocf61re78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1dm7rbo</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Am I tripping or is this shape weird?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndrjms2lc78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1dm7goz</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Probably the longest they've ever been 💚 I promise they're not dirty, just a little stained with cherry juice lol</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mh5xs53a78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1dm7991</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Todays Mani ☺️ 🩵💜</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqbo8fxb878d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1dm78vd</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Gel polish over hard UV gel</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm78vd/gel_polish_over_hard_uv_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1dm72jb</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Are you supposed to shape store bought fake nails? Don’t want to ruin them but they look clunky</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kb02f3r678d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1dm6tz7</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Product Recommendations for Basics </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm6tz7/product_recommendations_for_basics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1dm6qw3</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Accidentally split my nail with a razor - any tips on how to repair/regrowth care?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6qw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1dm6qve</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Want to try press on acrylics. Advice??</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm6qve/want_to_try_press_on_acrylics_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1dm6oy7</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These sparkly nails I got a while ago </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6oy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1dltuvs</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Ideas!</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://pin.it/KRJ9dHL36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1dm6c8n</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>My cousin did my nail art 🥰🥰🥰</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6c8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1dm6brg</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6brg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1dm5hmj</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>One of my first times painting my nails 🩷 do y’all like to paint your nails while they’re this short or do you prefer to grow them out first or does it matter?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujuw3j5mt68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1dm397p</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Regrowing nails after acrylics</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm397p/regrowing_nails_after_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1dm27hc</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>why do my nails curve like this?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm27hc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1dm0q05</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzdz0ibmq58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1dlyxxi</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I want to get my nails done to stop my skin picking disorder</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlyxxi/i_want_to_get_my_nails_done_to_stop_my_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1dlxy6q</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Hard Gel Removed &amp; Sporting Natural Nails- tips for strengthening them?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud03av10458d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1dm6621</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Builder gel (BIAB) with chrome - natural nail length. £45 in London ($57)</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6621</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1dm61i9</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Favorite press-ons ever</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm61i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1dm600x</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Going for a intense color combo</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm600x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1dm5uv3</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Berry Nails</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm5uv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1dm5tkx</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Tips for starting off with gel x</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm5tkx/tips_for_starting_off_with_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1dm58tj</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Bisexual clowns 🤡</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm58tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1dm58ho</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I only need the charms to last for one day, andomg I love these so much. </t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm58ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1dm3idw</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm3idw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1dm564p</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Is this a good nude for me?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2k4smszq68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1dm533s</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Mean Girl Nails</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yrk7llbq68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1dm4t9o</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Did Top coat too soon</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8dlwxu2o68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1dm4mbj</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Natural looking polish dyi</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k80cr0uim68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1dm4kse</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Reminds me of a MySpace layout</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm4kse</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1dm4bbn</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Piggy nails for my daughter. First one, I messed up the ear placement and he became evil 😅</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb4xk6a0k68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1dm4b7p</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Newbie gelx question</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dm4b7p/newbie_gelx_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1dm48bk</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>got my nails done for grad :)</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6mxxzqbj68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1dm3x2l</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Have A Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep7ii0isg68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1dm3pe9</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Please tell me they are not hideous.</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm3pe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1dm3m02</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Work in progress, dragon scales</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm3m02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1dlqatv</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pain After Pedicure </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dlqatv/pain_after_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1dm3epe</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>First time trying airbrush</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyo62f3hc68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1dm3bys</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Just got these done</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm3bys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1dm33sa</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>see through shimmery 🤩</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm33sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1dm2zda</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first summer mani ☀️🦞 </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42b0xkry868d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1dm2uws</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Cheerful little blueberries 🫐</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1led3zhy768d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1dm2ihd</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ideas for thumb and pinky for these 3d dragon nails I'm working on </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez9zz065568d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1dm237w</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Cheugy?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hegw8xbq168d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1dm1u93</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Celebritip nails</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm1u93</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1dm1kmg</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Sunflowers gnome set</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm1kmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1dm1c43</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I love sheerish colors with some shimmer. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8owrh7jqv58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1dm1anw</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Proud of my latest set!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm1anw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1dm17zg</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Eras tour nails</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm17zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1dm13hj</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Did these this morning!</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm13hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1dm11oz</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>new week, new set!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm11oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1dm0ym5</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Lighting struck⚡️</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0ym5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1dm0xtf</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Golden butterfly</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0xtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1dm0xf5</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>So proud of the sky blue nails I did yesterday</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0xf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1dm0wxj</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Butterfly nails🦋</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0wxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1dm0wis</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Structured manicure: ask anything!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0wis</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1dm0w5t</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time im able to grow them this long!! Hope they dont start breaking anytime soon. </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3lxjgo0s58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1dm0uvs</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Ocean blues🌊</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0uvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1dm0r8a</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Pearlescent ombré attempt</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85uyadmwq58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1dm0q9l</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Thanks to some overfilling while on vacation for the first time I have white unstained natural nails!</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az88zoeoq58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1dm0lnw</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>nail polish on gel x?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10nzfmomp58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1dm0hhj</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>how much would you charge/pay for this set?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g10t44ooo58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1dmgv5b</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Its official, the crackle is backle (found at Dollar General)</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j2fulqzy98d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1dmg2y5</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dmg2y5/holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1dmfk75</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Can anyone dupe this? Pfd moonlit</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chj61i0ui98d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1dme6ul</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out my new summer plate! </t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dme6ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1dmcxud</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>feeling very blue (da ba dee da ba di) 💙</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycrm0g8up88d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1dmcxnt</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>It Blue Me A Grey!  😉</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/OWqswle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1dmcl3z</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>my latest fav</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y10jdtg8m88d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1dmatvp</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatch Comparison Request </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dmatvp/swatch_comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1dmamrb</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>clean aestethics</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27uarvoe288d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1dmaleg</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Fun little rainbow skittle</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dmaleg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1dmaacw</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Watermelon 🍉 </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d56hp7sez78d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1dm8szj</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>My solstice x Midsommar look 🌻🌿☀️💐</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27k5j6hql78d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1dm8q86</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absolutely Ancient Claire's Offering </t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm8q86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1dm8aon</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>ISO Empty Kathleen &amp; Co bottles &amp;/OR brushes</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dm8aon/iso_empty_kathleen_co_bottles_or_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1dm87n9</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This month's colour </t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm87n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1dm7vd7</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Trans Pride Nails 🩵🩷🤍🩷🩵</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm7vd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1dm73p5</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Fair Maiden Tinties 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm73p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1dm6e72</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Seaside Kingdom ft. Mako (PPU 04/24)</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6e72</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1dm6cip</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Found my yellow!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm6cip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1dm64cw</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Golden Pig💛</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm64cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1dm4w83</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>I always see people done dirty on here… second time getting dip and extensions. Is this a good job?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm4w83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1dm4qpe</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm4qpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1dm4pyt</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Favorite POC swatchers on IG?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dm4pyt/favorite_poc_swatchers_on_ig/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1dm48is</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Feeling electric</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm48is</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1dm39p1</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Price at my local grocery store </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glzv3ibab68d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1dm2z0r</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Rose quartz Frenchies</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey33avov868d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1dm2x2a</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>First Lurid Lacquer Mani!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nahabrxf868d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1dm2w2e</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gimme your brown polish recommendations! </t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dm2w2e/gimme_your_brown_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1dm2fdr</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>First Watermarble for Pan Pride Flag</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm2fdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1dm1o0i</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Red polish similar to Gucci’s Rossa Ancora?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8ukuqpay58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1dm1acy</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Cancer the Crab 🦀 ft. My dogs fur</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm1acy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1dm15cl</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Easy nail polishes for a beginner?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dm15cl/easy_nail_polishes_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1dm0kfi</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>This is so prugly on me.</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm0kfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1dlzz8l</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Got my first set of dotting tools and was inspired to do some retro flowers</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlzz8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1dlznnl</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>natural 💅</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlznnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1dlz8j4</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Floral Bi Pride Nails 🌺🪻💙💅</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlz8j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1dly0mf</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>The longest I can handle before I tire of long nails</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dly0mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1dlwwaq</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smoothing base, transparent </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlwwaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1dlw37y</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>LynB formula makes it so easy to mix your own colors and I love it!</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlw37y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1dlws5h</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Mooncat “Selene”</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wzerqm7u48d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1dlwmqo</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Comparing Mooncat Siren's Deceit with Sassy Sauce Happy Ending</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlwmqo/comparing_mooncat_sirens_deceit_with_sassy_sauce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1dlw0rb</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈OG Gilbert Pride Flag🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlw0rb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1dlvv7o</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you have polish whose formula you hate, but you use it anyway because you love the results so much? </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzgm3ur7m48d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1dluupc</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lament </t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5enua3frc48d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1dlpx9a</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Nail Alternatives with Adhesive Allergies?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dlpx9a/nail_alternatives_with_adhesive_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1dlsjg4</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Turquoise for summer days</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yszkp1tum38d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1dlrmmp</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Glory goodness</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4wcx7g8b38d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1dlr5j2</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Christmas in June</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlr5j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1dm7dit</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm7dit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1dm4oif</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>I did these last Christmas. White Christmas themed</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bs4p091zm68d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1dm4dc5</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Banana nails 🍌🙈✨</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm4dc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1dm3pe6</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Custom nail set!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv3hqho0f68d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1dm2vp8</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>The Nail Bae 3D Gold Chrome Tutorial</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p3ly0eh4868d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1dm1hxr</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Sunflowers gnome set</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dm1hxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1dlz2mv</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Another Polygel set by me inspired by a Pinterest pic!</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jvp3a86d58d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1dlyowb</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Stuck lighting on this one⚡️</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlyowb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1dlyjzy</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Pushing up tiny daisies🌼</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nw6nbhx858d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1dlyj1k</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Sunrise chrome✨</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlyj1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1dlyfqc</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Ocean blue🌊</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlyfqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1dlutor</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>I’ve wanted to try the milk bath glitter look for a while</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlutor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1dlusnw</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>I’ve been on a Polygel kick recently!</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h44ps377c48d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1dltcay</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Daisy nails</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dltcay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1dlsh7d</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Fill and free style design</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dlsh7d</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>